<commit_message>
Updated the tests synthesis tables and notebook
</commit_message>
<xml_diff>
--- a/tests/validation/test_synthesis/Convergence_table_all.xlsx
+++ b/tests/validation/test_synthesis/Convergence_table_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="222">
   <si>
     <t>Boundary_conditions</t>
   </si>
@@ -124,21 +124,90 @@
     <t>Dirichlet</t>
   </si>
   <si>
-    <t>[0.16376200462748713, 0.05168516435187792, 0.026538599754443747, 0.018444334522280982, 0.004680847753865031, 0.0026658304312993622, 0.0017138741513224457]</t>
+    <t>[0.17381931481028523, 0.015704592474608387, 0.005088979181987203, 0.0008048788405363034, 0.00020967740067095124]</t>
   </si>
   <si>
     <t>Square</t>
   </si>
   <si>
+    <t>Maillage triangulaire</t>
+  </si>
+  <si>
+    <t>FE simulation of the 2D Poisson equation</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Triangles</t>
+  </si>
+  <si>
+    <t>SquareWithTriangles</t>
+  </si>
+  <si>
+    <t>[u'squareWithTriangles_1', u'squareWithTriangles_2', u'squareWithTriangles_3', u'squareWithTriangles_4', u'squareWithTriangles_5']</t>
+  </si>
+  <si>
+    <t>../../ressources/2DTriangles/</t>
+  </si>
+  <si>
+    <t>[5.385164807134504, 11.4455231422596, 22.49444375840399, 57.53259945457011, 114.6080276420461]</t>
+  </si>
+  <si>
+    <t>Unstructured_triangles</t>
+  </si>
+  <si>
+    <t>P1 FE</t>
+  </si>
+  <si>
+    <t>Finite elements</t>
+  </si>
+  <si>
+    <t>Poisson</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>[0.15982423136458235, 0.19209074180764232, 0.02588840408238014, 0.10154359684558502, 0.04012116796146481, 0.020355023119755823, 0.05256584074127857]</t>
+  </si>
+  <si>
+    <t>Cube</t>
+  </si>
+  <si>
+    <t>Tetrahedral mesh</t>
+  </si>
+  <si>
+    <t>FE simulation of the 3D Poisson equation</t>
+  </si>
+  <si>
+    <t>Tetrahedra</t>
+  </si>
+  <si>
+    <t>meshCubeWithTetrahedraFE</t>
+  </si>
+  <si>
+    <t>[u'meshCubeTetrahedra_0', u'meshCubeTetrahedra_1', u'meshCubeTetrahedra_2', u'meshCubeTetrahedra_3', u'meshCubeTetrahedra_4', u'meshCubeTetrahedra_5', u'meshCubeTetrahedra_6']</t>
+  </si>
+  <si>
+    <t>../../ressources/3DTetrahedra/</t>
+  </si>
+  <si>
+    <t>[4.198336453808407, 7.979112176485801, 9.43913067739236, 11.555497342463696, 14.995554238032435, 18.12667840184579, 23.18626317196864]</t>
+  </si>
+  <si>
+    <t>Unstructured_tetrahedra</t>
+  </si>
+  <si>
+    <t>[0.16376200462748672, 0.05168516435187811, 0.026538599754443802, 0.018444334522280822, 0.004680847753864083, 0.002665830431298749, 0.001713874151324999]</t>
+  </si>
+  <si>
     <t>2 points FV diffusion scheme</t>
   </si>
   <si>
     <t>FV simulation of the 2D Poisson equation</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Squares</t>
   </si>
   <si>
@@ -163,13 +232,7 @@
     <t>Finite volumes</t>
   </si>
   <si>
-    <t>Poisson</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>[0.07366496204246868, 0.037395159693908685, 0.02680097674922449, 0.02226683641491594, 0.020621909445644987, 0.01999007290664904]</t>
+    <t>[0.07366496204246864, 0.037395159693908345, 0.026800976749223833, 0.02226683641491438, 0.020621909445641656, 0.019990072906645822]</t>
   </si>
   <si>
     <t>SquareWithCheckerboardRefinement</t>
@@ -187,7 +250,7 @@
     <t>Non_conforming_checkerboard</t>
   </si>
   <si>
-    <t>[0.046208459926760315, 0.022852108867969657, 0.011943351423693894, 0.0062896232378350575, 0.003317293212916132, 0.0017485573538365896, 0.0009202671828575968]</t>
+    <t>[0.04620845992675999, 0.02285210886796976, 0.011943351423695231, 0.006289623237837, 0.003317293212917964, 0.0017485573538421413, 0.0009202671828583186]</t>
   </si>
   <si>
     <t>SquareWithLocRefSquares</t>
@@ -244,7 +307,7 @@
     <t>Regular_hexagons</t>
   </si>
   <si>
-    <t>[0.053029287545514815, 0.012950746721879576, 0.0032189644400791337, 0.0008035776793699633, 0.00020082180970142292]</t>
+    <t>[0.053029287545515065, 0.012950746721879921, 0.003218964440079805, 0.0008035776793705196, 0.0002008218097039779]</t>
   </si>
   <si>
     <t>SquareWithSquares</t>
@@ -262,31 +325,97 @@
     <t>Regular_squares</t>
   </si>
   <si>
-    <t>[0.04972168575894878, 0.04358040486275415, 0.021907135331019855, 0.011510133471143422, 0.007903217495358324]</t>
-  </si>
-  <si>
-    <t>Triangles</t>
-  </si>
-  <si>
-    <t>SquareWithTriangles</t>
-  </si>
-  <si>
-    <t>[u'squareWithTriangles_1', u'squareWithTriangles_2', u'squareWithTriangles_3', u'squareWithTriangles_4', u'squareWithTriangles_5']</t>
-  </si>
-  <si>
-    <t>../../ressources/2DTriangles/</t>
+    <t>[0.049721685758949134, 0.04358040486275415, 0.021907135331019553, 0.011510133471143921, 0.007903217495360328]</t>
   </si>
   <si>
     <t>[6.32455532033676, 14.966629547095765, 30.561413579872255, 80.13738203859668, 160.8477541030648]</t>
   </si>
   <si>
-    <t>Unstructured_triangles</t>
+    <t>[4.069145552990007, 5.5676107836145095, 6.524931809669063, 7.040279164662852]</t>
+  </si>
+  <si>
+    <t>FV simulation of the 3D Poisson equation</t>
+  </si>
+  <si>
+    <t>Cubes</t>
+  </si>
+  <si>
+    <t>CubeWithCheckerboardCubes</t>
+  </si>
+  <si>
+    <t>[u'cubeWithCheckerboardCubes_2x2x2', u'cubeWithCheckerboardCubes_4x4x4', u'cubeWithCheckerboardCubes_8x8x8', u'cubeWithCheckerboardCubes_16x16x16']</t>
+  </si>
+  <si>
+    <t>../../ressources/3DCheckerboard/</t>
+  </si>
+  <si>
+    <t>[3.3019272488946263, 6.6038544977892535, 13.207708995578502, 26.415417991157007]</t>
+  </si>
+  <si>
+    <t>Orange, BC violated. PB with mesh ?</t>
+  </si>
+  <si>
+    <t>[0.0068250597455885575, 0.001867093411123344, 0.0004894161427677622]</t>
+  </si>
+  <si>
+    <t>meshCubeWithCuboids3DFV</t>
+  </si>
+  <si>
+    <t>[11, 21, 41]</t>
+  </si>
+  <si>
+    <t>[10.999999999999996, 20.99999999999999, 40.99999999999999]</t>
+  </si>
+  <si>
+    <t>Regular_cubes</t>
+  </si>
+  <si>
+    <t>[0.24690168316230765, 0.08723262076393946, 0.0980747969963932, 0.09811268005866214, 0.07589566871761642, 0.050137919065019854, 0.05403048482079009]</t>
+  </si>
+  <si>
+    <t>CubeWithTetrahedra</t>
+  </si>
+  <si>
+    <t>[6.463304070095651, 12.767053944429668, 15.975222064844953, 19.685927060021815, 25.628849312676458, 30.56735094036983, 39.84292566537514]</t>
+  </si>
+  <si>
+    <t>[0.051827553080622826, 0.021394627131203593, 0.02257569506266233, 0.020599962007422246, 0.015254493191506473]</t>
+  </si>
+  <si>
+    <t>Triangular mesh, compact surface (no boundary)</t>
+  </si>
+  <si>
+    <t>FE simulation of the Poisson equation on a sphere</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>3DTriangles</t>
+  </si>
+  <si>
+    <t>SphereWithTriangles</t>
+  </si>
+  <si>
+    <t>[u'meshSphere_1', u'meshSphere_2', u'meshSphere_3', u'meshSphere_4', u'meshSphere_5']</t>
+  </si>
+  <si>
+    <t>../../ressources/3DSphere/</t>
+  </si>
+  <si>
+    <t>[16.970562748477143, 33.52610922848042, 51.36146415358503, 67.17142249498667, 103.79306335203714]</t>
+  </si>
+  <si>
+    <t>Unstructured_3D_triangles</t>
+  </si>
+  <si>
+    <t>Poisson-Beltrami</t>
   </si>
   <si>
     <t>Periodic</t>
   </si>
   <si>
-    <t>[1.533927991384892, 8.890973805007924, 35.385782506010244, 1.0, 1.016004783002024]</t>
+    <t>[1.029582795757373, 1.029841392959896, 1.030037809295173, 1.0304707455763509, 1.055321287842899]</t>
   </si>
   <si>
     <t>[0.003999999999999993, 0.004135416666666685, 0.004276041666666647, 0.006140624999999843, 0.006126302083332919]</t>
@@ -298,7 +427,7 @@
     <t>Constant pressure, divergence free velocity</t>
   </si>
   <si>
-    <t>[0.869128239273048, 1.0004732177138138, 1.016529317515402, 1.0127256622296852, 1.0058189006669649]</t>
+    <t>[0.8691282393639709, 1.0004732175377382, 1.0165293171989533, 1.0127256622030254, 1.0058188999669198]</t>
   </si>
   <si>
     <t>[1.2041199826559248, 1.806179973983887, 2.4082399653118496, 3.010299956639812, 3.612359947967774]</t>
@@ -307,13 +436,13 @@
     <t>Regular squares</t>
   </si>
   <si>
-    <t>[-7.465537090986128, -7.469006391415028, -7.156070843784089, -6.933848433076753, -6.41366914017297]</t>
-  </si>
-  <si>
-    <t>[-0.7908573951603067, -0.846133830947664, -0.9615975631519263, -1.1244759444424153, -1.329455101334318]</t>
-  </si>
-  <si>
-    <t>PStag no scaling</t>
+    <t>[-7.4655371447559995, -7.46900702556861, -7.156072747538284, -6.933847974673087, -6.413669137309963]</t>
+  </si>
+  <si>
+    <t>[-0.7908573948971233, -0.8461338255992907, -0.9615975356545877, -1.124475750153585, -1.329454301890515]</t>
+  </si>
+  <si>
+    <t>PStag scaling</t>
   </si>
   <si>
     <t>Implicit</t>
@@ -322,7 +451,7 @@
     <t>Wave system</t>
   </si>
   <si>
-    <t>[3.89333392224222, 33.21705189723093, 31.452685985108843, 1.0121061987727304]</t>
+    <t>[1.0441033752085294, 1.0349018998696151, 1.0326231824811367, 1.0926429773359316]</t>
   </si>
   <si>
     <t>[0.008648959937054891, 0.0069588209203450295, 0.012229806065635467, 0.00537674672742232]</t>
@@ -331,7 +460,7 @@
     <t>[990, 1897, 7497, 8714]</t>
   </si>
   <si>
-    <t>[0.9486278776337359, 1.0077566825602455, 1.005836506709227, 1.0050346369785461]</t>
+    <t>[0.9486278865568707, 1.0077566579539379, 1.005836762095434, 1.0050346389996483]</t>
   </si>
   <si>
     <t>[u'squareWithTriangles_1', u'squareWithTriangles_2', u'squareWithTriangles_3', u'squareWithTriangles_4']</t>
@@ -343,10 +472,10 @@
     <t>Unstructured triangles</t>
   </si>
   <si>
-    <t>[-6.946060830506312, -6.744294310101566, -6.629750851300356, -6.31186718496331]</t>
-  </si>
-  <si>
-    <t>[-0.9979741184405148, -1.0676611530522035, -1.230135590779631, -1.5643657162534277]</t>
+    <t>[-6.946077799953071, -6.744310775099525, -6.629707775993473, -6.311865880469129]</t>
+  </si>
+  <si>
+    <t>[-0.9979742132689434, -1.0676606920730933, -1.2301404695184956, -1.5643657824180908]</t>
   </si>
   <si>
     <t>Orange</t>
@@ -511,9 +640,6 @@
     <t>[1.4678583519379522, 1.5246189409582918, 1.5250673346782697]</t>
   </si>
   <si>
-    <t>Cubes</t>
-  </si>
-  <si>
     <t>CubeWithCubes</t>
   </si>
   <si>
@@ -539,12 +665,6 @@
   </si>
   <si>
     <t>[1.8234832327789146, 1.9568884938136755, 1.9880496573805357, 1.9921224192171922]</t>
-  </si>
-  <si>
-    <t>Tetrahedra</t>
-  </si>
-  <si>
-    <t>CubeWithTetrahedra</t>
   </si>
   <si>
     <t>[5, 11, 21, 26]</t>
@@ -908,7 +1028,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ18"/>
+  <dimension ref="A1:AJ24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1025,13 +1145,13 @@
     </row>
     <row r="2" spans="1:36">
       <c r="A2" s="1" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
       </c>
       <c r="C2" t="n">
-        <v>8.325439929962158</v>
+        <v>31.36970090866089</v>
       </c>
       <c r="D2" t="s"/>
       <c r="E2" t="s">
@@ -1102,7 +1222,7 @@
       </c>
       <c r="AE2" t="s"/>
       <c r="AF2" t="n">
-        <v>1.099715148758754</v>
+        <v>2.11982946328897</v>
       </c>
       <c r="AG2" t="s"/>
       <c r="AH2" t="s"/>
@@ -1115,13 +1235,13 @@
     </row>
     <row r="3" spans="1:36">
       <c r="A3" s="1" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="n">
-        <v>6.347608089447021</v>
+        <v>166.0481879711151</v>
       </c>
       <c r="D3" t="s"/>
       <c r="E3" t="s">
@@ -1130,41 +1250,41 @@
       <c r="F3" t="s"/>
       <c r="G3" t="s"/>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="K3" t="s">
         <v>40</v>
       </c>
       <c r="L3" t="s"/>
       <c r="M3" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="N3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="O3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P3" t="b">
         <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="R3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="S3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="T3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="U3" t="s"/>
       <c r="V3" t="s"/>
@@ -1192,12 +1312,12 @@
       </c>
       <c r="AE3" t="s"/>
       <c r="AF3" t="n">
-        <v>0.3500538307526435</v>
+        <v>0.9881680535318813</v>
       </c>
       <c r="AG3" t="s"/>
       <c r="AH3" t="s"/>
       <c r="AI3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ3" t="s">
         <v>50</v>
@@ -1205,17 +1325,17 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" s="1" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
       </c>
       <c r="C4" t="n">
-        <v>19.86432003974915</v>
+        <v>8.572041034698486</v>
       </c>
       <c r="D4" t="s"/>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s"/>
       <c r="G4" t="s"/>
@@ -1223,20 +1343,20 @@
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="K4" t="s">
         <v>40</v>
       </c>
       <c r="L4" t="s"/>
       <c r="M4" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="N4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="O4" t="n">
         <v>2</v>
@@ -1245,24 +1365,24 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="R4" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="S4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="T4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="U4" t="s"/>
       <c r="V4" t="s"/>
       <c r="W4" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="X4" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y4" t="s">
         <v>40</v>
@@ -1282,7 +1402,7 @@
       </c>
       <c r="AE4" t="s"/>
       <c r="AF4" t="n">
-        <v>0.936221110698956</v>
+        <v>1.099715148758559</v>
       </c>
       <c r="AG4" t="s"/>
       <c r="AH4" t="s"/>
@@ -1295,17 +1415,17 @@
     </row>
     <row r="5" spans="1:36">
       <c r="A5" s="1" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
       </c>
       <c r="C5" t="n">
-        <v>2.677490949630737</v>
+        <v>6.620848894119263</v>
       </c>
       <c r="D5" t="s"/>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s"/>
       <c r="G5" t="s"/>
@@ -1313,20 +1433,20 @@
         <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
         <v>40</v>
       </c>
       <c r="L5" t="s"/>
       <c r="M5" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="O5" t="n">
         <v>2</v>
@@ -1335,24 +1455,24 @@
         <v>1</v>
       </c>
       <c r="Q5" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="R5" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="S5" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="T5" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="U5" t="s"/>
       <c r="V5" t="s"/>
       <c r="W5" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="X5" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y5" t="s">
         <v>40</v>
@@ -1372,7 +1492,7 @@
       </c>
       <c r="AE5" t="s"/>
       <c r="AF5" t="n">
-        <v>-0.2073891905776415</v>
+        <v>0.3500538307526957</v>
       </c>
       <c r="AG5" t="s"/>
       <c r="AH5" t="s"/>
@@ -1385,17 +1505,17 @@
     </row>
     <row r="6" spans="1:36">
       <c r="A6" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
       </c>
       <c r="C6" t="n">
-        <v>3.250871896743774</v>
+        <v>21.06601786613464</v>
       </c>
       <c r="D6" t="s"/>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s"/>
       <c r="G6" t="s"/>
@@ -1403,20 +1523,20 @@
         <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="K6" t="s">
         <v>40</v>
       </c>
       <c r="L6" t="s"/>
       <c r="M6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="O6" t="n">
         <v>2</v>
@@ -1425,24 +1545,24 @@
         <v>1</v>
       </c>
       <c r="Q6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="R6" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="S6" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="T6" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="U6" t="s"/>
       <c r="V6" t="s"/>
       <c r="W6" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="X6" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y6" t="s">
         <v>40</v>
@@ -1462,7 +1582,7 @@
       </c>
       <c r="AE6" t="s"/>
       <c r="AF6" t="n">
-        <v>1.94163703307054</v>
+        <v>0.9362211106984839</v>
       </c>
       <c r="AG6" t="s"/>
       <c r="AH6" t="s"/>
@@ -1475,17 +1595,17 @@
     </row>
     <row r="7" spans="1:36">
       <c r="A7" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>35</v>
       </c>
       <c r="C7" t="n">
-        <v>1.420461177825928</v>
+        <v>2.427170038223267</v>
       </c>
       <c r="D7" t="s"/>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s"/>
       <c r="G7" t="s"/>
@@ -1493,20 +1613,20 @@
         <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="K7" t="s">
         <v>40</v>
       </c>
       <c r="L7" t="s"/>
       <c r="M7" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="N7" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="O7" t="n">
         <v>2</v>
@@ -1515,24 +1635,24 @@
         <v>1</v>
       </c>
       <c r="Q7" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="R7" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="S7" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="T7" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="U7" t="s"/>
       <c r="V7" t="s"/>
       <c r="W7" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="X7" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y7" t="s">
         <v>40</v>
@@ -1552,7 +1672,7 @@
       </c>
       <c r="AE7" t="s"/>
       <c r="AF7" t="n">
-        <v>2.009991317810532</v>
+        <v>-0.2073891905776415</v>
       </c>
       <c r="AG7" t="s"/>
       <c r="AH7" t="s"/>
@@ -1565,17 +1685,17 @@
     </row>
     <row r="8" spans="1:36">
       <c r="A8" s="1" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
       </c>
       <c r="C8" t="n">
-        <v>3.168046951293945</v>
+        <v>2.972708940505981</v>
       </c>
       <c r="D8" t="s"/>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F8" t="s"/>
       <c r="G8" t="s"/>
@@ -1583,20 +1703,20 @@
         <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="J8" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="K8" t="s">
         <v>40</v>
       </c>
       <c r="L8" t="s"/>
       <c r="M8" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="N8" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="O8" t="n">
         <v>2</v>
@@ -1605,24 +1725,24 @@
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="R8" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="S8" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="T8" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="U8" t="s"/>
       <c r="V8" t="s"/>
       <c r="W8" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="X8" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y8" t="s">
         <v>40</v>
@@ -1642,7 +1762,7 @@
       </c>
       <c r="AE8" t="s"/>
       <c r="AF8" t="n">
-        <v>0.6137798580984675</v>
+        <v>1.94163703307054</v>
       </c>
       <c r="AG8" t="s"/>
       <c r="AH8" t="s"/>
@@ -1655,95 +1775,87 @@
     </row>
     <row r="9" spans="1:36">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="C9" t="n">
-        <v>137.9682860374451</v>
-      </c>
-      <c r="D9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E9" t="s"/>
-      <c r="F9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H9" t="s"/>
-      <c r="I9" t="s"/>
-      <c r="J9" t="s"/>
+        <v>3.357578992843628</v>
+      </c>
+      <c r="D9" t="s"/>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" t="s"/>
+      <c r="G9" t="s"/>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
       <c r="K9" t="s">
-        <v>93</v>
-      </c>
-      <c r="L9" t="s">
-        <v>94</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="L9" t="s"/>
       <c r="M9" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="O9" t="n">
         <v>2</v>
       </c>
-      <c r="P9" t="s"/>
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q9" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="R9" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="S9" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="T9" t="s">
-        <v>96</v>
-      </c>
-      <c r="U9" t="s">
-        <v>97</v>
-      </c>
-      <c r="V9" t="s">
-        <v>98</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="U9" t="s"/>
+      <c r="V9" t="s"/>
       <c r="W9" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="X9" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y9" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>0.5</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="Z9" t="s"/>
       <c r="AA9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC9" t="b">
         <v>0</v>
       </c>
-      <c r="AB9" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC9" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD9" t="s"/>
-      <c r="AE9" t="n">
-        <v>0</v>
-      </c>
+      <c r="AD9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE9" t="s"/>
       <c r="AF9" t="n">
-        <v>-0.0002403281271210094</v>
-      </c>
-      <c r="AG9" t="n">
-        <v>-0.0002403281271210094</v>
-      </c>
-      <c r="AH9" t="n">
-        <v>0.0001169457565974146</v>
-      </c>
+        <v>2.009991317806771</v>
+      </c>
+      <c r="AG9" t="s"/>
+      <c r="AH9" t="s"/>
       <c r="AI9" t="n">
         <v>2</v>
       </c>
@@ -1753,287 +1865,267 @@
     </row>
     <row r="10" spans="1:36">
       <c r="A10" s="1" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="C10" t="n">
-        <v>388.8398141860962</v>
-      </c>
-      <c r="D10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E10" t="s"/>
-      <c r="F10" t="s">
+        <v>3.177055835723877</v>
+      </c>
+      <c r="D10" t="s"/>
+      <c r="E10" t="s">
         <v>103</v>
       </c>
-      <c r="G10" t="s">
+      <c r="F10" t="s"/>
+      <c r="G10" t="s"/>
+      <c r="H10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" t="s"/>
+      <c r="M10" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" t="n">
+        <v>2</v>
+      </c>
+      <c r="P10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" t="s">
+        <v>44</v>
+      </c>
+      <c r="S10" t="s">
         <v>104</v>
       </c>
-      <c r="H10" t="s"/>
-      <c r="I10" t="s"/>
-      <c r="J10" t="s"/>
-      <c r="K10" t="s">
-        <v>93</v>
-      </c>
-      <c r="L10" t="s">
-        <v>105</v>
-      </c>
-      <c r="M10" t="s">
-        <v>83</v>
-      </c>
-      <c r="N10" t="s">
-        <v>84</v>
-      </c>
-      <c r="O10" t="n">
-        <v>2</v>
-      </c>
-      <c r="P10" t="s"/>
-      <c r="Q10" t="s">
-        <v>106</v>
-      </c>
-      <c r="R10" t="s">
-        <v>86</v>
-      </c>
-      <c r="S10" t="s">
-        <v>107</v>
-      </c>
       <c r="T10" t="s">
-        <v>108</v>
-      </c>
-      <c r="U10" t="s">
-        <v>109</v>
-      </c>
-      <c r="V10" t="s">
-        <v>110</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="U10" t="s"/>
+      <c r="V10" t="s"/>
       <c r="W10" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="X10" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y10" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>0.5</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="Z10" t="s"/>
       <c r="AA10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC10" t="b">
         <v>0</v>
       </c>
-      <c r="AB10" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD10" t="s"/>
-      <c r="AE10" t="n">
-        <v>0</v>
-      </c>
+      <c r="AD10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE10" t="s"/>
       <c r="AF10" t="n">
-        <v>8.013775249613408e-05</v>
+        <v>0.6137798580984064</v>
       </c>
       <c r="AG10" t="s"/>
-      <c r="AH10" t="n">
-        <v>8.013775249613408e-05</v>
-      </c>
+      <c r="AH10" t="s"/>
       <c r="AI10" t="n">
         <v>2</v>
       </c>
       <c r="AJ10" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:36">
       <c r="A11" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="n">
+        <v>13.95365500450134</v>
+      </c>
+      <c r="D11" t="s"/>
+      <c r="E11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" t="s"/>
+      <c r="G11" t="s"/>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" t="s">
+        <v>106</v>
+      </c>
+      <c r="K11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" t="s"/>
+      <c r="M11" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" t="s">
+        <v>108</v>
+      </c>
+      <c r="O11" t="n">
+        <v>3</v>
+      </c>
+      <c r="P11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>109</v>
+      </c>
+      <c r="R11" t="s">
+        <v>110</v>
+      </c>
+      <c r="S11" t="s">
+        <v>111</v>
+      </c>
+      <c r="T11" t="s">
+        <v>77</v>
+      </c>
+      <c r="U11" t="s"/>
+      <c r="V11" t="s"/>
+      <c r="W11" t="s">
+        <v>70</v>
+      </c>
+      <c r="X11" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z11" t="s"/>
+      <c r="AA11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC11" t="b">
         <v>0</v>
       </c>
-      <c r="B11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" t="n">
-        <v>4.268468856811523</v>
-      </c>
-      <c r="D11" t="s"/>
-      <c r="E11" t="s"/>
-      <c r="F11" t="s">
+      <c r="AD11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE11" t="s"/>
+      <c r="AF11" t="n">
+        <v>-0.2601624714817707</v>
+      </c>
+      <c r="AG11" t="s"/>
+      <c r="AH11" t="s"/>
+      <c r="AI11" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ11" t="s">
         <v>112</v>
-      </c>
-      <c r="G11" t="s">
-        <v>113</v>
-      </c>
-      <c r="H11" t="s"/>
-      <c r="I11" t="s"/>
-      <c r="J11" t="s"/>
-      <c r="K11" t="s">
-        <v>93</v>
-      </c>
-      <c r="L11" t="s">
-        <v>114</v>
-      </c>
-      <c r="M11" t="s">
-        <v>115</v>
-      </c>
-      <c r="N11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O11" t="n">
-        <v>2</v>
-      </c>
-      <c r="P11" t="s"/>
-      <c r="Q11" t="s">
-        <v>116</v>
-      </c>
-      <c r="R11" t="s">
-        <v>44</v>
-      </c>
-      <c r="S11" t="s">
-        <v>117</v>
-      </c>
-      <c r="T11" t="s">
-        <v>115</v>
-      </c>
-      <c r="U11" t="s">
-        <v>118</v>
-      </c>
-      <c r="V11" t="s">
-        <v>119</v>
-      </c>
-      <c r="W11" t="s">
-        <v>120</v>
-      </c>
-      <c r="X11" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AA11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC11" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD11" t="s"/>
-      <c r="AE11" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>-3.487620212460162e-09</v>
-      </c>
-      <c r="AG11" t="n">
-        <v>-3.487620212460162e-09</v>
-      </c>
-      <c r="AH11" t="n">
-        <v>0.0001632754294598849</v>
-      </c>
-      <c r="AI11" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:36">
       <c r="A12" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="C12" t="n">
-        <v>8.631521940231323</v>
+        <v>24.51998209953308</v>
       </c>
       <c r="D12" t="s"/>
-      <c r="E12" t="s"/>
-      <c r="F12" t="s">
-        <v>121</v>
-      </c>
-      <c r="G12" t="s">
-        <v>122</v>
-      </c>
-      <c r="H12" t="s"/>
-      <c r="I12" t="s"/>
-      <c r="J12" t="s"/>
+      <c r="E12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" t="s"/>
+      <c r="G12" t="s"/>
+      <c r="H12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" t="s">
+        <v>106</v>
+      </c>
       <c r="K12" t="s">
-        <v>93</v>
-      </c>
-      <c r="L12" t="s">
-        <v>123</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="L12" t="s"/>
       <c r="M12" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="N12" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="O12" t="n">
-        <v>2</v>
-      </c>
-      <c r="P12" t="s"/>
+        <v>3</v>
+      </c>
+      <c r="P12" t="b">
+        <v>1</v>
+      </c>
       <c r="Q12" t="s">
-        <v>125</v>
-      </c>
-      <c r="R12" t="s">
-        <v>66</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="R12" t="s"/>
       <c r="S12" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="T12" t="s">
-        <v>127</v>
-      </c>
-      <c r="U12" t="s">
-        <v>128</v>
-      </c>
-      <c r="V12" t="s">
-        <v>129</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="U12" t="s"/>
+      <c r="V12" t="s"/>
       <c r="W12" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="X12" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y12" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>0.5</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="Z12" t="s"/>
       <c r="AA12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC12" t="b">
         <v>0</v>
       </c>
-      <c r="AB12" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC12" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD12" t="s"/>
-      <c r="AE12" t="s">
-        <v>40</v>
-      </c>
+      <c r="AD12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE12" t="s"/>
       <c r="AF12" t="n">
-        <v>-7.023350625076041e-06</v>
-      </c>
-      <c r="AG12" t="n">
-        <v>-3.148264048417944e-09</v>
-      </c>
-      <c r="AH12" t="n">
-        <v>-7.023350625076041e-06</v>
-      </c>
+        <v>2.002870871514143</v>
+      </c>
+      <c r="AG12" t="s"/>
+      <c r="AH12" t="s"/>
       <c r="AI12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ12" t="s">
         <v>50</v>
@@ -2041,95 +2133,89 @@
     </row>
     <row r="13" spans="1:36">
       <c r="A13" s="1" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>6.753997087478638</v>
+        <v>37.72716212272644</v>
       </c>
       <c r="D13" t="s"/>
-      <c r="E13" t="s"/>
-      <c r="F13" t="s">
-        <v>130</v>
-      </c>
-      <c r="G13" t="s">
-        <v>131</v>
-      </c>
-      <c r="H13" t="s"/>
-      <c r="I13" t="s"/>
-      <c r="J13" t="s"/>
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" t="s"/>
+      <c r="G13" t="s"/>
+      <c r="H13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" t="s">
+        <v>106</v>
+      </c>
       <c r="K13" t="s">
-        <v>93</v>
-      </c>
-      <c r="L13" t="s">
-        <v>132</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="L13" t="s"/>
       <c r="M13" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="N13" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="O13" t="n">
-        <v>2</v>
-      </c>
-      <c r="P13" t="s"/>
+        <v>3</v>
+      </c>
+      <c r="P13" t="b">
+        <v>1</v>
+      </c>
       <c r="Q13" t="s">
-        <v>134</v>
+        <v>57</v>
       </c>
       <c r="R13" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="S13" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="T13" t="s">
-        <v>136</v>
-      </c>
-      <c r="U13" t="s">
-        <v>137</v>
-      </c>
-      <c r="V13" t="s">
-        <v>138</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="U13" t="s"/>
+      <c r="V13" t="s"/>
       <c r="W13" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="X13" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y13" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>0.5</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="Z13" t="s"/>
       <c r="AA13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC13" t="b">
         <v>0</v>
       </c>
-      <c r="AB13" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC13" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD13" t="s"/>
-      <c r="AE13" t="s">
-        <v>40</v>
-      </c>
+      <c r="AD13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE13" t="s"/>
       <c r="AF13" t="n">
-        <v>-1.855096236805034e-11</v>
-      </c>
-      <c r="AG13" t="n">
-        <v>-1.855096236805034e-11</v>
-      </c>
-      <c r="AH13" t="n">
-        <v>0.000185386783872759</v>
-      </c>
+        <v>0.8110604778863585</v>
+      </c>
+      <c r="AG13" t="s"/>
+      <c r="AH13" t="s"/>
       <c r="AI13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ13" t="s">
         <v>50</v>
@@ -2137,95 +2223,89 @@
     </row>
     <row r="14" spans="1:36">
       <c r="A14" s="1" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="C14" t="n">
-        <v>9.09241509437561</v>
+        <v>9.205935001373291</v>
       </c>
       <c r="D14" t="s"/>
-      <c r="E14" t="s"/>
-      <c r="F14" t="s">
-        <v>139</v>
-      </c>
-      <c r="G14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H14" t="s"/>
-      <c r="I14" t="s"/>
-      <c r="J14" t="s"/>
+      <c r="E14" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" t="s"/>
+      <c r="G14" t="s"/>
+      <c r="H14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" t="s">
+        <v>122</v>
+      </c>
+      <c r="J14" t="s">
+        <v>123</v>
+      </c>
       <c r="K14" t="s">
-        <v>93</v>
-      </c>
-      <c r="L14" t="s">
-        <v>141</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="L14" t="s"/>
       <c r="M14" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="N14" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="O14" t="n">
         <v>2</v>
       </c>
-      <c r="P14" t="s"/>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
       <c r="Q14" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="R14" t="s">
-        <v>73</v>
+        <v>128</v>
       </c>
       <c r="S14" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="T14" t="s">
-        <v>145</v>
-      </c>
-      <c r="U14" t="s">
-        <v>146</v>
-      </c>
-      <c r="V14" t="s">
-        <v>147</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="U14" t="s"/>
+      <c r="V14" t="s"/>
       <c r="W14" t="s">
-        <v>120</v>
+        <v>47</v>
       </c>
       <c r="X14" t="s">
         <v>48</v>
       </c>
       <c r="Y14" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z14" t="n">
-        <v>0.5</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="Z14" t="s"/>
       <c r="AA14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC14" t="b">
         <v>0</v>
       </c>
-      <c r="AB14" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC14" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD14" t="s"/>
-      <c r="AE14" t="s">
-        <v>40</v>
-      </c>
+      <c r="AD14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE14" t="s"/>
       <c r="AF14" t="n">
-        <v>-8.564714050813453e-06</v>
-      </c>
-      <c r="AG14" t="n">
-        <v>-7.395998386565901e-10</v>
-      </c>
-      <c r="AH14" t="n">
-        <v>-8.564714050813453e-06</v>
-      </c>
+        <v>0.6091438624653882</v>
+      </c>
+      <c r="AG14" t="s"/>
+      <c r="AH14" t="s"/>
       <c r="AI14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ14" t="s">
         <v>50</v>
@@ -2233,67 +2313,69 @@
     </row>
     <row r="15" spans="1:36">
       <c r="A15" s="1" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="C15" t="n">
-        <v>6.354268789291382</v>
-      </c>
-      <c r="D15" t="s"/>
+        <v>48.67472195625305</v>
+      </c>
+      <c r="D15" t="s">
+        <v>133</v>
+      </c>
       <c r="E15" t="s"/>
       <c r="F15" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="G15" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="H15" t="s"/>
       <c r="I15" t="s"/>
       <c r="J15" t="s"/>
       <c r="K15" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="L15" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="M15" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="N15" t="s">
-        <v>151</v>
+        <v>98</v>
       </c>
       <c r="O15" t="n">
         <v>2</v>
       </c>
       <c r="P15" t="s"/>
       <c r="Q15" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="R15" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="S15" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="T15" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="U15" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="V15" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="W15" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="X15" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y15" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="Z15" t="n">
         <v>0.5</v>
@@ -2302,23 +2384,23 @@
         <v>0</v>
       </c>
       <c r="AB15" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="AC15" t="b">
         <v>1</v>
       </c>
       <c r="AD15" t="s"/>
-      <c r="AE15" t="s">
-        <v>40</v>
+      <c r="AE15" t="n">
+        <v>2</v>
       </c>
       <c r="AF15" t="n">
-        <v>-3.864405473494067e-05</v>
+        <v>-0.0002403283177935742</v>
       </c>
       <c r="AG15" t="n">
-        <v>-4.005028544584878e-10</v>
+        <v>-0.0002403283177935742</v>
       </c>
       <c r="AH15" t="n">
-        <v>-3.864405473494067e-05</v>
+        <v>0.0001169455589461346</v>
       </c>
       <c r="AI15" t="n">
         <v>2</v>
@@ -2329,67 +2411,69 @@
     </row>
     <row r="16" spans="1:36">
       <c r="A16" s="1" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="C16" t="n">
-        <v>4.388073921203613</v>
-      </c>
-      <c r="D16" t="s"/>
+        <v>138.2427699565887</v>
+      </c>
+      <c r="D16" t="s">
+        <v>145</v>
+      </c>
       <c r="E16" t="s"/>
       <c r="F16" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="G16" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H16" t="s"/>
       <c r="I16" t="s"/>
       <c r="J16" t="s"/>
       <c r="K16" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="L16" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="M16" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="N16" t="s">
-        <v>158</v>
+        <v>42</v>
       </c>
       <c r="O16" t="n">
         <v>2</v>
       </c>
       <c r="P16" t="s"/>
       <c r="Q16" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="R16" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="S16" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="T16" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="U16" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="V16" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="W16" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="X16" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y16" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="Z16" t="n">
         <v>0.5</v>
@@ -2398,101 +2482,101 @@
         <v>0</v>
       </c>
       <c r="AB16" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="AC16" t="b">
         <v>1</v>
       </c>
       <c r="AD16" t="s"/>
-      <c r="AE16" t="s">
-        <v>40</v>
+      <c r="AE16" t="n">
+        <v>2</v>
       </c>
       <c r="AF16" t="n">
-        <v>-8.25752331143273e-11</v>
-      </c>
-      <c r="AG16" t="n">
-        <v>-8.25752331143273e-11</v>
-      </c>
+        <v>8.013761360562131e-05</v>
+      </c>
+      <c r="AG16" t="s"/>
       <c r="AH16" t="n">
-        <v>9.710763747950686e-06</v>
+        <v>8.013761360562131e-05</v>
       </c>
       <c r="AI16" t="n">
         <v>2</v>
       </c>
       <c r="AJ16" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:36">
       <c r="A17" s="1" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="C17" t="n">
-        <v>13.37891101837158</v>
+        <v>3.91550087928772</v>
       </c>
       <c r="D17" t="s"/>
       <c r="E17" t="s"/>
       <c r="F17" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G17" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="H17" t="s"/>
       <c r="I17" t="s"/>
       <c r="J17" t="s"/>
       <c r="K17" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="L17" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="M17" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="N17" t="s">
-        <v>166</v>
+        <v>65</v>
       </c>
       <c r="O17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P17" t="s"/>
       <c r="Q17" t="s">
-        <v>167</v>
-      </c>
-      <c r="R17" t="s"/>
+        <v>159</v>
+      </c>
+      <c r="R17" t="s">
+        <v>67</v>
+      </c>
       <c r="S17" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="T17" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="U17" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="V17" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="W17" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="X17" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y17" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="AA17" t="b">
         <v>0</v>
       </c>
       <c r="AB17" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="AC17" t="b">
         <v>1</v>
@@ -2502,16 +2586,16 @@
         <v>40</v>
       </c>
       <c r="AF17" t="n">
-        <v>-3.26265785023925e-05</v>
+        <v>-3.487620212460162e-09</v>
       </c>
       <c r="AG17" t="n">
-        <v>-5.517038319237415e-11</v>
+        <v>-3.487620212460162e-09</v>
       </c>
       <c r="AH17" t="n">
-        <v>-3.26265785023925e-05</v>
+        <v>0.0001632754294598849</v>
       </c>
       <c r="AI17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AJ17" t="s">
         <v>50</v>
@@ -2519,74 +2603,76 @@
     </row>
     <row r="18" spans="1:36">
       <c r="A18" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="C18" t="n">
-        <v>82.49833798408508</v>
+        <v>6.973340034484863</v>
       </c>
       <c r="D18" t="s"/>
       <c r="E18" t="s"/>
       <c r="F18" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="G18" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H18" t="s"/>
       <c r="I18" t="s"/>
       <c r="J18" t="s"/>
       <c r="K18" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="L18" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="M18" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="N18" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="O18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P18" t="s"/>
       <c r="Q18" t="s">
-        <v>177</v>
-      </c>
-      <c r="R18" t="s"/>
+        <v>168</v>
+      </c>
+      <c r="R18" t="s">
+        <v>87</v>
+      </c>
       <c r="S18" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="T18" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="U18" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="V18" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="W18" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="X18" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="Y18" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="AA18" t="b">
         <v>0</v>
       </c>
       <c r="AB18" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="AC18" t="b">
         <v>1</v>
@@ -2596,18 +2682,590 @@
         <v>40</v>
       </c>
       <c r="AF18" t="n">
+        <v>-7.023350625076041e-06</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>-3.148264048417944e-09</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>-7.023350625076041e-06</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36">
+      <c r="A19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" t="n">
+        <v>6.204435110092163</v>
+      </c>
+      <c r="D19" t="s"/>
+      <c r="E19" t="s"/>
+      <c r="F19" t="s">
+        <v>173</v>
+      </c>
+      <c r="G19" t="s">
+        <v>174</v>
+      </c>
+      <c r="H19" t="s"/>
+      <c r="I19" t="s"/>
+      <c r="J19" t="s"/>
+      <c r="K19" t="s">
+        <v>136</v>
+      </c>
+      <c r="L19" t="s">
+        <v>175</v>
+      </c>
+      <c r="M19" t="s">
+        <v>64</v>
+      </c>
+      <c r="N19" t="s">
+        <v>176</v>
+      </c>
+      <c r="O19" t="n">
+        <v>2</v>
+      </c>
+      <c r="P19" t="s"/>
+      <c r="Q19" t="s">
+        <v>177</v>
+      </c>
+      <c r="R19" t="s">
+        <v>75</v>
+      </c>
+      <c r="S19" t="s">
+        <v>178</v>
+      </c>
+      <c r="T19" t="s">
+        <v>179</v>
+      </c>
+      <c r="U19" t="s">
+        <v>180</v>
+      </c>
+      <c r="V19" t="s">
+        <v>181</v>
+      </c>
+      <c r="W19" t="s">
+        <v>163</v>
+      </c>
+      <c r="X19" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD19" t="s"/>
+      <c r="AE19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>-1.855096236805034e-11</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>-1.855096236805034e-11</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>0.000185386783872759</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" t="n">
+        <v>7.821051836013794</v>
+      </c>
+      <c r="D20" t="s"/>
+      <c r="E20" t="s"/>
+      <c r="F20" t="s">
+        <v>182</v>
+      </c>
+      <c r="G20" t="s">
+        <v>183</v>
+      </c>
+      <c r="H20" t="s"/>
+      <c r="I20" t="s"/>
+      <c r="J20" t="s"/>
+      <c r="K20" t="s">
+        <v>136</v>
+      </c>
+      <c r="L20" t="s">
+        <v>184</v>
+      </c>
+      <c r="M20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N20" t="s">
+        <v>185</v>
+      </c>
+      <c r="O20" t="n">
+        <v>2</v>
+      </c>
+      <c r="P20" t="s"/>
+      <c r="Q20" t="s">
+        <v>186</v>
+      </c>
+      <c r="R20" t="s">
+        <v>94</v>
+      </c>
+      <c r="S20" t="s">
+        <v>187</v>
+      </c>
+      <c r="T20" t="s">
+        <v>188</v>
+      </c>
+      <c r="U20" t="s">
+        <v>189</v>
+      </c>
+      <c r="V20" t="s">
+        <v>190</v>
+      </c>
+      <c r="W20" t="s">
+        <v>163</v>
+      </c>
+      <c r="X20" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD20" t="s"/>
+      <c r="AE20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>-8.564714050813453e-06</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>-7.395998386565901e-10</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>-8.564714050813453e-06</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36">
+      <c r="A21" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" t="n">
+        <v>6.330248832702637</v>
+      </c>
+      <c r="D21" t="s"/>
+      <c r="E21" t="s"/>
+      <c r="F21" t="s">
+        <v>191</v>
+      </c>
+      <c r="G21" t="s">
+        <v>192</v>
+      </c>
+      <c r="H21" t="s"/>
+      <c r="I21" t="s"/>
+      <c r="J21" t="s"/>
+      <c r="K21" t="s">
+        <v>136</v>
+      </c>
+      <c r="L21" t="s">
+        <v>193</v>
+      </c>
+      <c r="M21" t="s">
+        <v>64</v>
+      </c>
+      <c r="N21" t="s">
+        <v>194</v>
+      </c>
+      <c r="O21" t="n">
+        <v>2</v>
+      </c>
+      <c r="P21" t="s"/>
+      <c r="Q21" t="s">
+        <v>99</v>
+      </c>
+      <c r="R21" t="s">
+        <v>100</v>
+      </c>
+      <c r="S21" t="s">
+        <v>195</v>
+      </c>
+      <c r="T21" t="s">
+        <v>139</v>
+      </c>
+      <c r="U21" t="s">
+        <v>196</v>
+      </c>
+      <c r="V21" t="s">
+        <v>197</v>
+      </c>
+      <c r="W21" t="s">
+        <v>163</v>
+      </c>
+      <c r="X21" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD21" t="s"/>
+      <c r="AE21" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>-3.864405473494067e-05</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>-4.005028544584878e-10</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>-3.864405473494067e-05</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36">
+      <c r="A22" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" t="n">
+        <v>4.3265061378479</v>
+      </c>
+      <c r="D22" t="s"/>
+      <c r="E22" t="s"/>
+      <c r="F22" t="s">
+        <v>198</v>
+      </c>
+      <c r="G22" t="s">
+        <v>199</v>
+      </c>
+      <c r="H22" t="s"/>
+      <c r="I22" t="s"/>
+      <c r="J22" t="s"/>
+      <c r="K22" t="s">
+        <v>136</v>
+      </c>
+      <c r="L22" t="s">
+        <v>200</v>
+      </c>
+      <c r="M22" t="s">
+        <v>41</v>
+      </c>
+      <c r="N22" t="s">
+        <v>201</v>
+      </c>
+      <c r="O22" t="n">
+        <v>2</v>
+      </c>
+      <c r="P22" t="s"/>
+      <c r="Q22" t="s">
+        <v>149</v>
+      </c>
+      <c r="R22" t="s">
+        <v>44</v>
+      </c>
+      <c r="S22" t="s">
+        <v>202</v>
+      </c>
+      <c r="T22" t="s">
+        <v>151</v>
+      </c>
+      <c r="U22" t="s">
+        <v>203</v>
+      </c>
+      <c r="V22" t="s">
+        <v>204</v>
+      </c>
+      <c r="W22" t="s">
+        <v>163</v>
+      </c>
+      <c r="X22" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA22" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD22" t="s"/>
+      <c r="AE22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>-8.25752331143273e-11</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>-8.25752331143273e-11</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>9.710763747950686e-06</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36">
+      <c r="A23" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" t="n">
+        <v>11.58602809906006</v>
+      </c>
+      <c r="D23" t="s"/>
+      <c r="E23" t="s"/>
+      <c r="F23" t="s">
+        <v>205</v>
+      </c>
+      <c r="G23" t="s">
+        <v>206</v>
+      </c>
+      <c r="H23" t="s"/>
+      <c r="I23" t="s"/>
+      <c r="J23" t="s"/>
+      <c r="K23" t="s">
+        <v>136</v>
+      </c>
+      <c r="L23" t="s">
+        <v>207</v>
+      </c>
+      <c r="M23" t="s">
+        <v>107</v>
+      </c>
+      <c r="N23" t="s">
+        <v>208</v>
+      </c>
+      <c r="O23" t="n">
+        <v>3</v>
+      </c>
+      <c r="P23" t="s"/>
+      <c r="Q23" t="s">
+        <v>209</v>
+      </c>
+      <c r="R23" t="s"/>
+      <c r="S23" t="s">
+        <v>210</v>
+      </c>
+      <c r="T23" t="s">
+        <v>211</v>
+      </c>
+      <c r="U23" t="s">
+        <v>212</v>
+      </c>
+      <c r="V23" t="s">
+        <v>213</v>
+      </c>
+      <c r="W23" t="s">
+        <v>163</v>
+      </c>
+      <c r="X23" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="AA23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD23" t="s"/>
+      <c r="AE23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>-3.26265785023925e-05</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>-5.517038319237415e-11</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>-3.26265785023925e-05</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36">
+      <c r="A24" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" t="n">
+        <v>74.72236084938049</v>
+      </c>
+      <c r="D24" t="s"/>
+      <c r="E24" t="s"/>
+      <c r="F24" t="s">
+        <v>214</v>
+      </c>
+      <c r="G24" t="s">
+        <v>215</v>
+      </c>
+      <c r="H24" t="s"/>
+      <c r="I24" t="s"/>
+      <c r="J24" t="s"/>
+      <c r="K24" t="s">
+        <v>136</v>
+      </c>
+      <c r="L24" t="s">
+        <v>216</v>
+      </c>
+      <c r="M24" t="s">
+        <v>55</v>
+      </c>
+      <c r="N24" t="s">
+        <v>119</v>
+      </c>
+      <c r="O24" t="n">
+        <v>3</v>
+      </c>
+      <c r="P24" t="s"/>
+      <c r="Q24" t="s">
+        <v>217</v>
+      </c>
+      <c r="R24" t="s"/>
+      <c r="S24" t="s">
+        <v>218</v>
+      </c>
+      <c r="T24" t="s">
+        <v>219</v>
+      </c>
+      <c r="U24" t="s">
+        <v>220</v>
+      </c>
+      <c r="V24" t="s">
+        <v>221</v>
+      </c>
+      <c r="W24" t="s">
+        <v>163</v>
+      </c>
+      <c r="X24" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="AA24" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD24" t="s"/>
+      <c r="AE24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF24" t="n">
         <v>-1.117834915917594e-11</v>
       </c>
-      <c r="AG18" t="n">
+      <c r="AG24" t="n">
         <v>-1.117834915917594e-11</v>
       </c>
-      <c r="AH18" t="n">
+      <c r="AH24" t="n">
         <v>1.719676889825437e-06</v>
       </c>
-      <c r="AI18" t="n">
+      <c r="AI24" t="n">
         <v>3</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AJ24" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>